<commit_message>
adding info MICS and LSMS
</commit_message>
<xml_diff>
--- a/input/data_recap.xlsx
+++ b/input/data_recap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Dropbox\PhD thesis\chapitre_3\predicting-undernutrition-rate-Nigeria\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A076A06C-0835-4397-A3FF-725806264A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18180AE7-00D7-473F-9E73-078F167928AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72455A7D-9D48-4A83-99C5-0F3C079B3C59}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Year</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>remarks</t>
+  </si>
+  <si>
+    <t>GIS data not available</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
+  </si>
+  <si>
+    <t>Anthropometric data not available</t>
+  </si>
+  <si>
+    <t>2010 - 2011</t>
   </si>
 </sst>
 </file>
@@ -449,7 +461,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2005</v>
       </c>
@@ -765,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2006</v>
       </c>
@@ -783,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>2007</v>
       </c>
@@ -800,8 +812,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2008</v>
       </c>
@@ -819,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2009</v>
       </c>
@@ -837,9 +852,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6">
-        <v>2010</v>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B22" s="7">
         <v>0</v>
@@ -855,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2011</v>
       </c>
@@ -872,8 +887,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>2012</v>
       </c>
@@ -891,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2013</v>
       </c>
@@ -909,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2014</v>
       </c>
@@ -927,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>2015</v>
       </c>
@@ -945,9 +963,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
-        <v>2016</v>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B28" s="5">
         <v>0</v>
@@ -963,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2017</v>
       </c>
@@ -981,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>2018</v>
       </c>
@@ -999,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>2019</v>
       </c>
@@ -1017,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2020</v>
       </c>
@@ -1035,7 +1053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>2021</v>
       </c>
@@ -1052,8 +1070,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2022</v>
       </c>
@@ -1071,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>2023</v>
       </c>
@@ -1089,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2024</v>
       </c>

</xml_diff>